<commit_message>
Added button to download raw data points in MS spreadsheet
</commit_message>
<xml_diff>
--- a/build/Rose.xlsx
+++ b/build/Rose.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="10" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,40 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="22">
-  <si>
-    <t xml:space="preserve">k </t>
-  </si>
-  <si>
-    <t xml:space="preserve">E₁</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E₂</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E₃</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E₄</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E₅</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M₁</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M₂</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M₃</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M₄</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M₅</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="11">
   <si>
     <t xml:space="preserve">k</t>
   </si>
@@ -176,7 +143,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -199,8 +166,8 @@
   </sheetPr>
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -469,14 +436,14 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -702,15 +669,15 @@
   </sheetPr>
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M18" activeCellId="0" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -937,14 +904,14 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1206,14 +1173,14 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1475,44 +1442,44 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1744,14 +1711,14 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2013,14 +1980,14 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2289,37 +2256,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2551,14 +2518,14 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2820,14 +2787,14 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>

</xml_diff>